<commit_message>
Parte da View da aula 05
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -42,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Retornar a partir do minuto 52:00 - Construindo as Models</t>
+Retornar a partir do minuto 1:25:00 - Construindo as Models</t>
         </r>
       </text>
     </comment>
@@ -309,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +374,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9.5"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -479,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -528,6 +535,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1113,7 +1121,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">

</xml_diff>

<commit_message>
06 - Apresentando o Entity Framework Core
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
@@ -15,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Usuário do Windows</author>
-  </authors>
-  <commentList>
-    <comment ref="A8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Usuário do Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Retornar a partir do minuto 1:25:00 - Construindo as Models</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -307,8 +278,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,19 +333,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="9.5"/>
@@ -383,7 +341,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -523,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,7 +500,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -547,6 +515,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -554,7 +525,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -592,9 +563,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -629,7 +600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -664,7 +635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -837,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,24 +829,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
       <c r="Q1" s="10" t="s">
         <v>76</v>
       </c>
@@ -920,10 +891,10 @@
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="7" t="s">
         <v>19</v>
       </c>
@@ -942,16 +913,16 @@
       <c r="U3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="V3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="20"/>
+      <c r="W3" s="21"/>
       <c r="X3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -968,7 +939,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R4" s="6" t="s">
@@ -976,7 +947,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -993,13 +964,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="21"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1025,7 +996,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1045,7 +1016,7 @@
       <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1064,7 +1035,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1121,7 +1092,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="18" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1420,7 +1391,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 07 - Identity 3.0
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,6 +15,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuário do Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Usuário do Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assistido até o minuto 22:28</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -137,9 +166,6 @@
     <t>12 - Tornando o domínio mapeavel para o banco de dados - [58 min]</t>
   </si>
   <si>
-    <t>13 - Criando a camada de Dados - [01h17 min]</t>
-  </si>
-  <si>
     <t>14 - Criando a camada de Aplicação - [1h20 min]</t>
   </si>
   <si>
@@ -197,9 +223,6 @@
     <t>17 - Finalizando as funcionalidades de Apresentação - [3h41 min]</t>
   </si>
   <si>
-    <t>18 - Tratamento e Log de Erros e Auditoria no MVC - [01h59 min]</t>
-  </si>
-  <si>
     <t>19 - Camada de Serviços ASPNET WebAPI - [3h51 min]</t>
   </si>
   <si>
@@ -209,9 +232,6 @@
     <t>21 - Angular Startup Template - [01h05 min]</t>
   </si>
   <si>
-    <t>22 - Rotas e recursos de navegação do Angular - [02h01 min]</t>
-  </si>
-  <si>
     <t>CNetCoreNG-AS</t>
   </si>
   <si>
@@ -273,13 +293,22 @@
   </si>
   <si>
     <t>NÃO</t>
+  </si>
+  <si>
+    <t>13 - Criando a camada de Dados - [1h17 min]</t>
+  </si>
+  <si>
+    <t>18 - Tratamento e Log de Erros e Auditoria no MVC - [1h59 min]</t>
+  </si>
+  <si>
+    <t>22 - Rotas e recursos de navegação do Angular - [2h01 min]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,8 +369,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -457,9 +505,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -488,6 +533,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,8 +549,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -525,7 +573,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -563,9 +611,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,7 +648,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +683,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -808,11 +856,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,106 +877,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="I1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="Q1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="I1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="Q1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="R3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="T3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="V3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="W3" s="22"/>
+      <c r="X3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" s="21"/>
-      <c r="X3" s="7" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -939,135 +987,135 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>78</v>
+      <c r="Q4" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="6" t="s">
-        <v>79</v>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="16">
+        <v>80</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="15">
         <v>43307</v>
       </c>
-      <c r="Q6" s="14" t="s">
-        <v>81</v>
+      <c r="Q6" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="4"/>
-      <c r="Q7" s="15"/>
+      <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="4"/>
@@ -1079,33 +1127,33 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -1115,16 +1163,16 @@
         <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
@@ -1134,16 +1182,16 @@
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4"/>
@@ -1153,206 +1201,206 @@
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>66</v>
+        <v>47</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>68</v>
+        <v>49</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>69</v>
+        <v>50</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>71</v>
+        <v>52</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>72</v>
+        <v>53</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>73</v>
+        <v>54</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="4"/>
@@ -1391,6 +1439,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 07 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -383,7 +383,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,12 +402,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -498,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -548,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,7 +851,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1093,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">

</xml_diff>

<commit_message>
Aula 08 - Primeira Parte
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -21,7 +21,7 @@
     <author>Usuário do Windows</author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Assistido até o minuto 22:28</t>
+Assistido até o minuto 19:50
+</t>
         </r>
       </text>
     </comment>
@@ -308,7 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,14 +363,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="9.5"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -383,7 +376,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -543,6 +541,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -851,7 +850,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,24 +867,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
       <c r="Q1" s="9" t="s">
         <v>73</v>
       </c>
@@ -930,10 +929,10 @@
       <c r="L3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="22"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
@@ -952,16 +951,16 @@
       <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="22"/>
+      <c r="W3" s="21"/>
       <c r="X3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -978,7 +977,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="22" t="s">
         <v>77</v>
       </c>
       <c r="R4" s="5" t="s">
@@ -986,7 +985,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1003,13 +1002,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1035,7 +1034,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1055,7 +1054,7 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1074,7 +1073,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1093,7 +1092,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1112,7 +1111,7 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1131,7 +1130,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">

</xml_diff>

<commit_message>
Aula 08 - Ferramentas Front-End
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
   </bookViews>
@@ -15,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Usuário do Windows</author>
-  </authors>
-  <commentList>
-    <comment ref="A10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Usuário do Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Assistido até o minuto 22:28</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -307,8 +278,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,29 +332,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="9.5"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,12 +352,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -498,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -532,7 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -548,9 +491,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -573,7 +513,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -611,9 +551,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -648,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,7 +623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,24 +817,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
       <c r="Q1" s="9" t="s">
         <v>73</v>
       </c>
@@ -939,10 +879,10 @@
       <c r="L3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="22"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
@@ -961,16 +901,16 @@
       <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="22"/>
+      <c r="W3" s="21"/>
       <c r="X3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -987,7 +927,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="22" t="s">
         <v>77</v>
       </c>
       <c r="R4" s="5" t="s">
@@ -995,7 +935,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1012,13 +952,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1044,7 +984,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1064,7 +1004,7 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1083,7 +1023,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1102,7 +1042,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1121,7 +1061,7 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1140,7 +1080,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1439,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 09 - Parte 1
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Aula assistida até 15:06</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +366,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +399,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -442,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -492,6 +545,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -796,11 +850,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1134,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1379,6 +1433,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
1 - Alterações do nome da pasta 2 - Aula 09 Parte 01
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -533,6 +533,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -545,7 +546,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -854,7 +854,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,24 +871,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="I1" s="19" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="I1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
       <c r="Q1" s="9" t="s">
         <v>73</v>
       </c>
@@ -933,10 +933,10 @@
       <c r="L3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="21"/>
+      <c r="N3" s="22"/>
       <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
@@ -955,10 +955,10 @@
       <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="20" t="s">
+      <c r="V3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="21"/>
+      <c r="W3" s="22"/>
       <c r="X3" s="6" t="s">
         <v>19</v>
       </c>
@@ -981,7 +981,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="23" t="s">
         <v>77</v>
       </c>
       <c r="R4" s="5" t="s">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="22"/>
+      <c r="Q5" s="23"/>
       <c r="R5" s="5" t="s">
         <v>76</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">

</xml_diff>

<commit_message>
Aula 09 - Finalizado
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Aula assistida até 15:06</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,21 +332,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,12 +352,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -495,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -533,7 +480,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -850,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,24 +817,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
       <c r="Q1" s="9" t="s">
         <v>73</v>
       </c>
@@ -933,10 +879,10 @@
       <c r="L3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="22"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
@@ -955,10 +901,10 @@
       <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="22"/>
+      <c r="W3" s="21"/>
       <c r="X3" s="6" t="s">
         <v>19</v>
       </c>
@@ -981,7 +927,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="22" t="s">
         <v>77</v>
       </c>
       <c r="R4" s="5" t="s">
@@ -1006,7 +952,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="5" t="s">
         <v>76</v>
       </c>
@@ -1134,7 +1080,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1433,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 10 - Criação dos 3 primeiros projetos Domain
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+minuto 25:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 10 - Até o minuto 53
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="27795" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
     <author>Alexandro e Fabiana</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-minuto 25:00</t>
+minuto 53:00</t>
         </r>
       </text>
     </comment>
@@ -312,7 +307,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -598,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -670,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -846,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 10 - Até o minuto 1:30:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -41,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-minuto 53:00</t>
+minuto 1:30:00</t>
         </r>
       </text>
     </comment>
@@ -842,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 11 - Até o minut 39:30
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 39:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 11 - Até o minuto 1:27:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="27795" windowHeight="12405"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="27795" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
     <author>Alexandro e Fabiana</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 39:00</t>
+Até o minuto 1:27:00</t>
         </r>
       </text>
     </comment>
@@ -312,7 +307,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -598,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -670,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -847,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 11 - Até o minuto 2:21:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="27795" windowHeight="12345"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="27795" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 1:27:00</t>
+Até o minuto 2:21:00</t>
         </r>
       </text>
     </comment>
@@ -842,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 11 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="420" windowWidth="27795" windowHeight="12285"/>
   </bookViews>
@@ -15,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 2:21:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -307,8 +278,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -555,7 +513,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -593,9 +551,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,7 +623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -838,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1118,7 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1421,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 12 - Até o minuto 40:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="27795" windowHeight="12285"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,6 +15,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuário do Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Usuário do Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 40:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -278,8 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +360,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -513,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -551,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,11 +838,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1421,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 12 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -842,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">

</xml_diff>

<commit_message>
Aula 13 - Até o minuto 48:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -21,7 +21,7 @@
     <author>Usuário do Windows</author>
   </authors>
   <commentList>
-    <comment ref="A15" authorId="0">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 40:00</t>
+Até o minuto 48:00</t>
         </r>
       </text>
     </comment>
@@ -842,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 13 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
@@ -15,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Usuário do Windows</author>
-  </authors>
-  <commentList>
-    <comment ref="A16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Usuário do Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 48:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -307,8 +278,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -555,7 +513,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -593,9 +551,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,7 +623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -838,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1156,7 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1421,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 14 - Até o minuto 30:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 27:30</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,7 +843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 14 - Até o minuto 45:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 30:00</t>
+Até o minuto 45:00</t>
         </r>
       </text>
     </comment>
@@ -847,7 +847,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 14 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 45:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,7 +796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
@@ -1222,7 +1175,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1426,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 15 - Até 1:00:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 1:00:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 15 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 1:00:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1194,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1426,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 16 - Até o minuto 14:43
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
@@ -20,6 +15,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuário do Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="A19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Usuário do Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 14:43</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -278,8 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +360,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -513,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -551,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,7 +838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
@@ -1379,6 +1421,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 16 - Até o minuto 59:43
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -41,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 14:43</t>
+Até o minuto 59:43</t>
         </r>
       </text>
     </comment>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,10 +987,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
@@ -1010,10 +1010,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>79</v>
@@ -1036,10 +1036,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="4"/>
@@ -1056,10 +1056,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="4"/>
@@ -1075,10 +1075,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="4"/>
@@ -1094,10 +1094,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="4"/>
@@ -1113,10 +1113,10 @@
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="4"/>
@@ -1132,10 +1132,10 @@
         <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -1151,10 +1151,10 @@
         <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
@@ -1170,10 +1170,10 @@
         <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4"/>
@@ -1189,10 +1189,10 @@
         <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="4"/>
@@ -1208,10 +1208,10 @@
         <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="4"/>
@@ -1227,10 +1227,10 @@
         <v>62</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="4"/>
@@ -1246,10 +1246,10 @@
         <v>63</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="4"/>

</xml_diff>

<commit_message>
Aula 16 - Até 1:23:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -29,7 +29,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Usuário do Windows:</t>
         </r>
@@ -38,10 +38,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 59:43</t>
+Até o minuto 1:23:43</t>
         </r>
       </text>
     </comment>
@@ -365,14 +365,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -842,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Até o minuto 2:20:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <author>Usuário do Windows</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +46,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 1:23:43</t>
+Até o minuto 2:20:00</t>
         </r>
       </text>
     </comment>
@@ -307,7 +312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,7 +560,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -593,9 +598,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,7 +670,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -841,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aula 16 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Usuário do Windows</author>
-  </authors>
-  <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Usuário do Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 2:20:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1213,7 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1270,7 +1223,7 @@
         <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>80</v>
@@ -1426,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Até o minuto 20
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 20:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 17 - Até o minuto 1:01:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 20:00</t>
+Até o minuto 1:01:00</t>
         </r>
       </text>
     </comment>
@@ -847,7 +847,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 17 - Até o minuto 2:42:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 1:01:00</t>
+Até o minuto 2:42:00</t>
         </r>
       </text>
     </comment>
@@ -847,7 +847,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 17 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 2:42:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,7 +796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
@@ -1279,7 +1232,7 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1426,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 18 - Até 0 minuto 36:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
@@ -20,6 +15,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuário do Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Usuário do Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 36:01</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -278,8 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +360,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -513,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -551,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,11 +838,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1421,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 18 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -15,40 +15,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Usuário do Windows</author>
-  </authors>
-  <commentList>
-    <comment ref="A21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Usuário do Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 36:01</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -308,7 +274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,19 +326,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -838,7 +791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
@@ -1293,7 +1246,7 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1421,7 +1374,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 19 - Até o minuto 1:00:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,6 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandro e Fabiana</author>
+  </authors>
+  <commentList>
+    <comment ref="A22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandro e Fabiana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Até o minuto 1:00:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -279,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -796,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1298,7 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1379,6 +1426,7 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 19 - Até 1:15:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alexandro\Aprendizado\Eduardo Pires\AspNetCoreVimeo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="12225"/>
   </bookViews>
@@ -26,7 +21,7 @@
     <author>Alexandro e Fabiana</author>
   </authors>
   <commentList>
-    <comment ref="A22" authorId="0" shapeId="0">
+    <comment ref="A22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 1:00:00</t>
+Até o minuto 1:15:00</t>
         </r>
       </text>
     </comment>
@@ -312,7 +307,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,7 +555,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -598,9 +593,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -670,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -847,7 +842,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 19 - Até 2:06
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 1:00:00</t>
+Até o minuto 2:06:00</t>
         </r>
       </text>
     </comment>
@@ -847,7 +847,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 19 - Até 2:45:00
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Até o minuto 2:06:00</t>
+Até o minuto 2:45:00</t>
         </r>
       </text>
     </comment>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 19 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -20,40 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandro e Fabiana</author>
-  </authors>
-  <commentList>
-    <comment ref="A22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandro e Fabiana:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Até o minuto 2:45:00</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
@@ -313,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,19 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1270,7 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1426,7 +1379,6 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 20 - Término
</commit_message>
<xml_diff>
--- a/Planejamento para assistir aula.xlsx
+++ b/Planejamento para assistir aula.xlsx
@@ -800,7 +800,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1289,7 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="3" t="s">

</xml_diff>